<commit_message>
Update for missing report & 405 error fix
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CraigVD\Downloads\ReportsProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5343449C-E153-4E06-8BCB-D3DF7681E08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D42C31-2099-43E9-AD5C-5EA84AEDB5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{083CF9A5-5B14-47B2-B195-9E0881BAB7D5}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="232">
   <si>
     <t>AldertV@exim.co.za</t>
   </si>
@@ -741,10 +741,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -773,14 +781,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1113,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B005DF3-5EC7-478B-87D6-579D5B0545A8}">
-  <dimension ref="A1:B883"/>
+  <dimension ref="A1:B886"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A875" workbookViewId="0">
+      <selection activeCell="C898" sqref="C898"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8189,12 +8200,41 @@
         <v>108</v>
       </c>
     </row>
+    <row r="884" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A884" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B884" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="885" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A885" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B885" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="886" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A886" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B886" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D882" xr:uid="{9B005DF3-5EC7-478B-87D6-579D5B0545A8}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B883">
       <sortCondition ref="B1:B882"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="A884" r:id="rId1" xr:uid="{B51B1E91-75E2-4F1E-ABF1-A81535C69112}"/>
+    <hyperlink ref="A885" r:id="rId2" xr:uid="{47053D57-F555-4702-A24F-78FBF74F7924}"/>
+    <hyperlink ref="A886" r:id="rId3" xr:uid="{76452A3C-AA3A-47FF-920B-627F5FFF8961}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>